<commit_message>
3/18 somethings are working
</commit_message>
<xml_diff>
--- a/Scripts/loanDetails.xlsx
+++ b/Scripts/loanDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\golu6\Downloads\CMS\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E89BB8-C5BB-46AC-A275-BFBCB751737A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0DC36F-A237-4A6D-8380-40D9155A640D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="70">
   <si>
     <t>LOAN ID</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>pending</t>
+  </si>
+  <si>
+    <t>20230317DE1703</t>
   </si>
   <si>
     <t>Loan ID</t>
@@ -272,9 +275,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -556,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL2"/>
+  <dimension ref="A1:AL4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -768,6 +772,160 @@
         <v>42</v>
       </c>
     </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>5000</v>
+      </c>
+      <c r="C3">
+        <v>0.05</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3">
+        <v>437.5</v>
+      </c>
+      <c r="I3">
+        <v>5250</v>
+      </c>
+      <c r="J3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3">
+        <v>1.575</v>
+      </c>
+      <c r="M3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" t="s">
+        <v>42</v>
+      </c>
+      <c r="V3" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" t="s">
+        <v>42</v>
+      </c>
+      <c r="X3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>120000</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3">
+        <v>45002</v>
+      </c>
+      <c r="F4" s="3">
+        <v>45002</v>
+      </c>
+      <c r="G4" s="3">
+        <v>45368</v>
+      </c>
+      <c r="H4">
+        <v>10050</v>
+      </c>
+      <c r="I4">
+        <v>120600</v>
+      </c>
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4">
+        <v>0.1</v>
+      </c>
+      <c r="L4">
+        <v>120.6</v>
+      </c>
+      <c r="M4">
+        <v>12</v>
+      </c>
+      <c r="O4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" t="s">
+        <v>42</v>
+      </c>
+      <c r="S4" t="s">
+        <v>42</v>
+      </c>
+      <c r="T4" t="s">
+        <v>42</v>
+      </c>
+      <c r="U4" t="s">
+        <v>42</v>
+      </c>
+      <c r="V4" t="s">
+        <v>42</v>
+      </c>
+      <c r="W4" t="s">
+        <v>42</v>
+      </c>
+      <c r="X4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -775,10 +933,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -789,82 +947,82 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="O1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="P1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="R1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="S1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="U1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="V1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="W1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="X1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Y1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.4">
@@ -906,6 +1064,88 @@
       </c>
       <c r="M2" s="2">
         <v>45331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="3">
+        <v>44994</v>
+      </c>
+      <c r="C3" s="3">
+        <v>45025</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45055</v>
+      </c>
+      <c r="E3" s="3">
+        <v>45086</v>
+      </c>
+      <c r="F3" s="3">
+        <v>45116</v>
+      </c>
+      <c r="G3" s="3">
+        <v>45147</v>
+      </c>
+      <c r="H3" s="3">
+        <v>45178</v>
+      </c>
+      <c r="I3" s="3">
+        <v>45208</v>
+      </c>
+      <c r="J3" s="3">
+        <v>45239</v>
+      </c>
+      <c r="K3" s="3">
+        <v>45269</v>
+      </c>
+      <c r="L3" s="3">
+        <v>45300</v>
+      </c>
+      <c r="M3" s="3">
+        <v>45331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="3">
+        <v>44996</v>
+      </c>
+      <c r="C4" s="3">
+        <v>45033</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45063</v>
+      </c>
+      <c r="E4" s="3">
+        <v>45094</v>
+      </c>
+      <c r="F4" s="3">
+        <v>45124</v>
+      </c>
+      <c r="G4" s="3">
+        <v>45155</v>
+      </c>
+      <c r="H4" s="3">
+        <v>45186</v>
+      </c>
+      <c r="I4" s="3">
+        <v>45216</v>
+      </c>
+      <c r="J4" s="3">
+        <v>45247</v>
+      </c>
+      <c r="K4" s="3">
+        <v>45277</v>
+      </c>
+      <c r="L4" s="3">
+        <v>45308</v>
+      </c>
+      <c r="M4" s="3">
+        <v>45339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LAST TIME for now
</commit_message>
<xml_diff>
--- a/Scripts/loanDetails.xlsx
+++ b/Scripts/loanDetails.xlsx
@@ -16,9 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -59,8 +60,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,8 +407,8 @@
   </sheetPr>
   <dimension ref="A1:AL9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
@@ -613,119 +614,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>20230225RA2502</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="D2" t="n">
-        <v>12</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2023-03-09</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2023-03-09</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2024-03-09</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>437.5</v>
-      </c>
-      <c r="I2" t="n">
-        <v>5250</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Rahul</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>0.03</t>
-        </is>
-      </c>
-      <c r="L2" t="n">
-        <v>1.575</v>
-      </c>
-      <c r="M2" t="n">
-        <v>12</v>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-    </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -854,13 +743,13 @@
       <c r="D4" t="n">
         <v>12</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="2" t="n">
         <v>45002</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="2" t="n">
         <v>45002</v>
       </c>
-      <c r="G4" s="3" t="n">
+      <c r="G4" s="2" t="n">
         <v>45368</v>
       </c>
       <c r="H4" t="n">
@@ -966,7 +855,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-03-09</t>
+          <t>2024-03-09</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -1057,9 +946,171 @@
         </is>
       </c>
     </row>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>20230319SH1903</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>200</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>45017</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>45017</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>45078</v>
+      </c>
+      <c r="H6" t="n">
+        <v>105</v>
+      </c>
+      <c r="I6" t="n">
+        <v>210</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Manager</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>20230319SH1903</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>200</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>45017</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>45017</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>45078</v>
+      </c>
+      <c r="H7" t="n">
+        <v>105</v>
+      </c>
+      <c r="I7" t="n">
+        <v>210</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Manager</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>20230319SH1903</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>200</v>
+      </c>
+      <c r="C8" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>45017</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>45017</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>45078</v>
+      </c>
+      <c r="H8" t="n">
+        <v>105</v>
+      </c>
+      <c r="I8" t="n">
+        <v>210</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Manager</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>2</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
     <row r="9"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1072,10 +1123,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
@@ -1217,47 +1268,18 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>20230225RA2502</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="n">
-        <v>44994</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>45025</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>45055</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>45086</v>
-      </c>
-      <c r="F2" s="3" t="n">
-        <v>45116</v>
-      </c>
-      <c r="G2" s="3" t="n">
-        <v>45147</v>
-      </c>
-      <c r="H2" s="3" t="n">
-        <v>45178</v>
-      </c>
-      <c r="I2" s="3" t="n">
-        <v>45208</v>
-      </c>
-      <c r="J2" s="3" t="n">
-        <v>45239</v>
-      </c>
-      <c r="K2" s="3" t="n">
-        <v>45269</v>
-      </c>
-      <c r="L2" s="3" t="n">
-        <v>45300</v>
-      </c>
-      <c r="M2" s="3" t="n">
-        <v>45331</v>
-      </c>
+      <c r="B2" s="2" t="n"/>
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="2" t="n"/>
+      <c r="E2" s="2" t="n"/>
+      <c r="F2" s="2" t="n"/>
+      <c r="G2" s="2" t="n"/>
+      <c r="H2" s="2" t="n"/>
+      <c r="I2" s="2" t="n"/>
+      <c r="J2" s="2" t="n"/>
+      <c r="K2" s="2" t="n"/>
+      <c r="L2" s="2" t="n"/>
+      <c r="M2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1265,40 +1287,40 @@
           <t>20230225RA2502</t>
         </is>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="2" t="n">
         <v>44994</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="2" t="n">
         <v>45025</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="2" t="n">
         <v>45055</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="2" t="n">
         <v>45086</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="2" t="n">
         <v>45116</v>
       </c>
-      <c r="G3" s="3" t="n">
+      <c r="G3" s="2" t="n">
         <v>45147</v>
       </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" s="2" t="n">
         <v>45178</v>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="2" t="n">
         <v>45208</v>
       </c>
-      <c r="J3" s="3" t="n">
+      <c r="J3" s="2" t="n">
         <v>45239</v>
       </c>
-      <c r="K3" s="3" t="n">
+      <c r="K3" s="2" t="n">
         <v>45269</v>
       </c>
-      <c r="L3" s="3" t="n">
+      <c r="L3" s="2" t="n">
         <v>45300</v>
       </c>
-      <c r="M3" s="3" t="n">
+      <c r="M3" s="2" t="n">
         <v>45331</v>
       </c>
     </row>
@@ -1308,40 +1330,40 @@
           <t>20230317DE1703</t>
         </is>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="2" t="n">
         <v>44996</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="2" t="n">
         <v>45033</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="2" t="n">
         <v>45063</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="2" t="n">
         <v>45094</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="2" t="n">
         <v>45124</v>
       </c>
-      <c r="G4" s="3" t="n">
+      <c r="G4" s="2" t="n">
         <v>45155</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="2" t="n">
         <v>45186</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="2" t="n">
         <v>45216</v>
       </c>
-      <c r="J4" s="3" t="n">
+      <c r="J4" s="2" t="n">
         <v>45247</v>
       </c>
-      <c r="K4" s="3" t="n">
+      <c r="K4" s="2" t="n">
         <v>45277</v>
       </c>
-      <c r="L4" s="3" t="n">
+      <c r="L4" s="2" t="n">
         <v>45308</v>
       </c>
-      <c r="M4" s="3" t="n">
+      <c r="M4" s="2" t="n">
         <v>45339</v>
       </c>
     </row>
@@ -1351,41 +1373,95 @@
           <t>20230225RA2502</t>
         </is>
       </c>
-      <c r="B5" s="4" t="n">
-        <v>44994</v>
-      </c>
-      <c r="C5" s="4" t="n">
-        <v>45025</v>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>45055</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <v>45086</v>
-      </c>
-      <c r="F5" s="4" t="n">
-        <v>45116</v>
-      </c>
-      <c r="G5" s="4" t="n">
-        <v>45147</v>
-      </c>
-      <c r="H5" s="4" t="n">
-        <v>45178</v>
-      </c>
-      <c r="I5" s="4" t="n">
-        <v>45208</v>
-      </c>
-      <c r="J5" s="4" t="n">
-        <v>45239</v>
-      </c>
-      <c r="K5" s="4" t="n">
-        <v>45269</v>
-      </c>
-      <c r="L5" s="4" t="n">
-        <v>45300</v>
-      </c>
-      <c r="M5" s="4" t="n">
-        <v>45331</v>
+      <c r="B5" s="3" t="n">
+        <v>45360</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>45391</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>45421</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>45452</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>45482</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>45513</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>45544</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>45574</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>45605</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <v>45635</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>45666</v>
+      </c>
+      <c r="M5" s="3" t="n">
+        <v>45697</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <v>45725</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>20230319SH1903</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2023-05-01</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2023-06-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>20230319SH1903</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2023-04-01</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2023-04-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>20230319SH1903</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2023-04-01</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2023-05-01</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>